<commit_message>
Test User and Head
</commit_message>
<xml_diff>
--- a/docs/Excel_sprint1.xlsx
+++ b/docs/Excel_sprint1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sprint1\git-group-repository-group-3-sec-2-v-2\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{592D4D6E-B802-42BD-849A-ADAB2E9CA726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D359F6D0-770A-4165-B7C8-DC963F9E5743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -467,9 +467,6 @@
 https://sesec2group3.cpkkuhost.com</t>
   </si>
   <si>
-    <t>SESec2Group3</t>
-  </si>
-  <si>
     <t xml:space="preserve">DATE: </t>
   </si>
   <si>
@@ -555,6 +552,9 @@
   </si>
   <si>
     <t>เนื่องจากหน้าก่อนหน้าเทสไม่สำเร็จ จึงส่งผลต่อหน้านี้ด้วย</t>
+  </si>
+  <si>
+    <t>SESec2Group3_Sprint1</t>
   </si>
 </sst>
 </file>
@@ -977,6 +977,42 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1029,42 +1065,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2448,6 +2448,128 @@
     </xdr:pic>
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>273050</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>635000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="image4.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22504314-3D0D-C796-4F01-369E05A74BD8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="19634200" y="0"/>
+          <a:ext cx="3289300" cy="4876800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>273050</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>635000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F162D8E-9A64-E35F-5FA2-B4483096B987}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="19634200" y="0"/>
+          <a:ext cx="3289300" cy="4876800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2692,12 +2814,12 @@
         <v>5</v>
       </c>
       <c r="I3" s="23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
-      <c r="J3" s="44" t="s">
+      <c r="J3" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="45"/>
+      <c r="K3" s="57"/>
     </row>
     <row r="4" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3696,7 +3818,7 @@
   <dimension ref="A1:I997"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="53" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.95"/>
@@ -3712,14 +3834,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="1.55">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="56"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="68"/>
       <c r="I1" s="20" t="s">
         <v>8</v>
       </c>
@@ -3739,54 +3861,54 @@
       <c r="A3" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="57" t="s">
-        <v>141</v>
+      <c r="B3" s="69" t="s">
+        <v>170</v>
       </c>
-      <c r="C3" s="53"/>
+      <c r="C3" s="65"/>
       <c r="D3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="52"/>
-      <c r="F3" s="45"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="57"/>
     </row>
     <row r="4" spans="1:9" ht="44.5" customHeight="1" x14ac:dyDescent="0.95">
       <c r="A4" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="58"/>
-      <c r="C4" s="53"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="65"/>
       <c r="D4" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="59">
+      <c r="E4" s="71">
         <f ca="1">TODAY()</f>
-        <v>45700</v>
+        <v>45713</v>
       </c>
-      <c r="F4" s="45"/>
+      <c r="F4" s="57"/>
     </row>
     <row r="5" spans="1:9" ht="36.5" customHeight="1" x14ac:dyDescent="0.95">
       <c r="A5" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="52"/>
-      <c r="C5" s="53"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="65"/>
       <c r="D5" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="60" t="s">
+      <c r="E5" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="45"/>
+      <c r="F5" s="57"/>
     </row>
     <row r="6" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="52"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="45"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="57"/>
     </row>
     <row r="7" spans="1:9" ht="32.5" customHeight="1" x14ac:dyDescent="0.95">
       <c r="A7" s="8"/>
@@ -3817,7 +3939,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="107" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="58" t="s">
         <v>124</v>
       </c>
       <c r="B9" s="25" t="s">
@@ -3830,14 +3952,14 @@
         <v>109</v>
       </c>
       <c r="E9" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="F9" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="F9" s="26" t="s">
-        <v>163</v>
-      </c>
     </row>
     <row r="10" spans="1:9" ht="93.5" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A10" s="47"/>
+      <c r="A10" s="59"/>
       <c r="B10" s="27" t="s">
         <v>25</v>
       </c>
@@ -3851,11 +3973,11 @@
         <v>111</v>
       </c>
       <c r="F10" s="26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="146" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A11" s="47"/>
+      <c r="A11" s="59"/>
       <c r="B11" s="25" t="s">
         <v>26</v>
       </c>
@@ -3869,11 +3991,11 @@
         <v>112</v>
       </c>
       <c r="F11" s="26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="106.5" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A12" s="47"/>
+      <c r="A12" s="59"/>
       <c r="B12" s="25" t="s">
         <v>27</v>
       </c>
@@ -3892,7 +4014,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="125" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A13" s="47"/>
+      <c r="A13" s="59"/>
       <c r="B13" s="25" t="s">
         <v>28</v>
       </c>
@@ -3911,7 +4033,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="88" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A14" s="47"/>
+      <c r="A14" s="59"/>
       <c r="B14" s="25" t="s">
         <v>29</v>
       </c>
@@ -3922,7 +4044,7 @@
         <v>137</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F14" s="26" t="str">
         <f t="shared" si="0"/>
@@ -3930,7 +4052,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="156.5" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A15" s="47"/>
+      <c r="A15" s="59"/>
       <c r="B15" s="25" t="s">
         <v>30</v>
       </c>
@@ -3941,7 +4063,7 @@
         <v>119</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F15" s="26" t="str">
         <f t="shared" si="0"/>
@@ -3949,7 +4071,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="219.5" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A16" s="47"/>
+      <c r="A16" s="59"/>
       <c r="B16" s="25" t="s">
         <v>31</v>
       </c>
@@ -3960,7 +4082,7 @@
         <v>121</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F16" s="26" t="str">
         <f t="shared" si="0"/>
@@ -3968,7 +4090,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="105.5" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A17" s="47"/>
+      <c r="A17" s="59"/>
       <c r="B17" s="25" t="s">
         <v>32</v>
       </c>
@@ -3979,7 +4101,7 @@
         <v>126</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F17" s="26" t="str">
         <f t="shared" si="0"/>
@@ -3987,18 +4109,18 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="104" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A18" s="47"/>
+      <c r="A18" s="59"/>
       <c r="B18" s="25" t="s">
         <v>33</v>
       </c>
       <c r="C18" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="D18" s="35" t="s">
         <v>155</v>
       </c>
-      <c r="D18" s="35" t="s">
-        <v>156</v>
-      </c>
       <c r="E18" s="35" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F18" s="26" t="str">
         <f t="shared" ref="F18" si="1">IF(E18="","",IF(D18=E18,"Pass","Fail"))</f>
@@ -4006,19 +4128,19 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="2.5" hidden="1" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A19" s="47"/>
+      <c r="A19" s="59"/>
     </row>
     <row r="20" spans="1:6" ht="32.5" hidden="1" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A20" s="47"/>
+      <c r="A20" s="59"/>
     </row>
     <row r="21" spans="1:6" ht="42" hidden="1" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A21" s="47"/>
+      <c r="A21" s="59"/>
     </row>
     <row r="22" spans="1:6" ht="1" hidden="1" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A22" s="47"/>
+      <c r="A22" s="59"/>
     </row>
     <row r="23" spans="1:6" ht="3" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A23" s="48"/>
+      <c r="A23" s="60"/>
     </row>
     <row r="24" spans="1:6" ht="21.5" customHeight="1" x14ac:dyDescent="0.95"/>
     <row r="25" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.95">
@@ -4029,7 +4151,7 @@
       <c r="F25" s="31"/>
     </row>
     <row r="26" spans="1:6" ht="89.5" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A26" s="49" t="s">
+      <c r="A26" s="61" t="s">
         <v>138</v>
       </c>
       <c r="B26" s="37" t="s">
@@ -4042,14 +4164,14 @@
         <v>109</v>
       </c>
       <c r="E26" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="F26" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="F26" s="26" t="s">
-        <v>163</v>
-      </c>
     </row>
     <row r="27" spans="1:6" ht="213.5" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A27" s="50"/>
+      <c r="A27" s="62"/>
       <c r="B27" s="37" t="s">
         <v>35</v>
       </c>
@@ -4062,17 +4184,17 @@
       <c r="E27" s="39" t="s">
         <v>127</v>
       </c>
-      <c r="F27" s="68" t="str">
-        <f t="shared" ref="F27:F32" si="2">IF(E27="","",IF(D27=E27,"Pass","Fail"))</f>
+      <c r="F27" s="49" t="str">
+        <f t="shared" ref="F27" si="2">IF(E27="","",IF(D27=E27,"Pass","Fail"))</f>
         <v>Pass</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="95.5" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A28" s="50"/>
-      <c r="B28" s="66" t="s">
+      <c r="A28" s="62"/>
+      <c r="B28" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="67" t="s">
+      <c r="C28" s="48" t="s">
         <v>135</v>
       </c>
       <c r="D28" s="40" t="s">
@@ -4081,17 +4203,17 @@
       <c r="E28" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="F28" s="73" t="s">
-        <v>163</v>
+      <c r="F28" s="54" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="115.5" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A29" s="50"/>
-      <c r="B29" s="72" t="s">
+      <c r="A29" s="62"/>
+      <c r="B29" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C29" s="41" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D29" s="40" t="s">
         <v>130</v>
@@ -4099,30 +4221,30 @@
       <c r="E29" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="F29" s="74" t="s">
-        <v>163</v>
+      <c r="F29" s="55" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="99" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A30" s="50"/>
-      <c r="B30" s="69" t="s">
+      <c r="A30" s="62"/>
+      <c r="B30" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="70" t="s">
+      <c r="C30" s="51" t="s">
         <v>129</v>
       </c>
-      <c r="D30" s="71" t="s">
+      <c r="D30" s="52" t="s">
         <v>128</v>
       </c>
-      <c r="E30" s="71" t="s">
+      <c r="E30" s="52" t="s">
         <v>128</v>
       </c>
       <c r="F30" s="30" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="129" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A31" s="50"/>
+      <c r="A31" s="62"/>
       <c r="B31" s="37" t="s">
         <v>39</v>
       </c>
@@ -4136,16 +4258,16 @@
         <v>132</v>
       </c>
       <c r="F31" s="26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="161" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A32" s="50"/>
+      <c r="A32" s="62"/>
       <c r="B32" s="37" t="s">
         <v>40</v>
       </c>
       <c r="C32" s="30" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D32" s="34" t="s">
         <v>133</v>
@@ -4154,47 +4276,47 @@
         <v>133</v>
       </c>
       <c r="F32" s="26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A33" s="50"/>
+      <c r="A33" s="62"/>
       <c r="B33" s="37" t="s">
         <v>123</v>
       </c>
       <c r="C33" s="30" t="s">
+        <v>163</v>
+      </c>
+      <c r="D33" s="34" t="s">
         <v>164</v>
       </c>
-      <c r="D33" s="34" t="s">
-        <v>165</v>
-      </c>
       <c r="E33" s="34" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F33" s="26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="76" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A34" s="50"/>
+      <c r="A34" s="62"/>
       <c r="B34" s="37" t="s">
         <v>134</v>
       </c>
       <c r="C34" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="D34" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="D34" s="34" t="s">
-        <v>167</v>
-      </c>
       <c r="E34" s="26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F34" s="26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="92.5" hidden="1" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A35" s="50"/>
+      <c r="A35" s="62"/>
       <c r="B35" s="31"/>
       <c r="C35" s="31"/>
       <c r="D35" s="31"/>
@@ -4202,7 +4324,7 @@
       <c r="F35" s="31"/>
     </row>
     <row r="36" spans="1:6" ht="78" hidden="1" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A36" s="50"/>
+      <c r="A36" s="62"/>
       <c r="B36" s="31"/>
       <c r="C36" s="31"/>
       <c r="D36" s="31"/>
@@ -4210,7 +4332,7 @@
       <c r="F36" s="31"/>
     </row>
     <row r="37" spans="1:6" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A37" s="50"/>
+      <c r="A37" s="62"/>
       <c r="B37" s="31"/>
       <c r="C37" s="31"/>
       <c r="D37" s="31"/>
@@ -4218,7 +4340,7 @@
       <c r="F37" s="31"/>
     </row>
     <row r="38" spans="1:6" ht="82.5" hidden="1" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A38" s="50"/>
+      <c r="A38" s="62"/>
       <c r="B38" s="31"/>
       <c r="C38" s="31"/>
       <c r="D38" s="31"/>
@@ -4226,7 +4348,7 @@
       <c r="F38" s="31"/>
     </row>
     <row r="39" spans="1:6" ht="0.5" customHeight="1" x14ac:dyDescent="1.25">
-      <c r="A39" s="50"/>
+      <c r="A39" s="62"/>
       <c r="B39" s="32"/>
       <c r="C39" s="32"/>
       <c r="D39" s="32"/>
@@ -4234,7 +4356,7 @@
       <c r="F39" s="32"/>
     </row>
     <row r="40" spans="1:6" ht="1" customHeight="1" x14ac:dyDescent="1.25">
-      <c r="A40" s="50"/>
+      <c r="A40" s="62"/>
       <c r="B40" s="32"/>
       <c r="C40" s="32"/>
       <c r="D40" s="32"/>
@@ -4242,7 +4364,7 @@
       <c r="F40" s="32"/>
     </row>
     <row r="41" spans="1:6" ht="1.5" customHeight="1" x14ac:dyDescent="1.25">
-      <c r="A41" s="50"/>
+      <c r="A41" s="62"/>
       <c r="B41" s="32"/>
       <c r="C41" s="32"/>
       <c r="D41" s="32"/>
@@ -6930,43 +7052,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="63">
+      <c r="A1" s="44">
         <v>45693</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="46" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="51.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="44">
+        <v>45694</v>
+      </c>
+      <c r="B2" s="46" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="51.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="63">
-        <v>45694</v>
+    <row r="3" spans="1:2" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="44">
+        <v>45695</v>
       </c>
-      <c r="B2" s="65" t="s">
+      <c r="B3" s="45" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="63">
-        <v>45695</v>
-      </c>
-      <c r="B3" s="64" t="s">
-        <v>160</v>
-      </c>
-    </row>
     <row r="4" spans="1:2" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="63">
+      <c r="A4" s="44">
         <v>45698</v>
       </c>
-      <c r="B4" s="64" t="s">
-        <v>160</v>
+      <c r="B4" s="45" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="63">
+      <c r="A5" s="44">
         <v>45699</v>
       </c>
-      <c r="B5" s="64" t="s">
-        <v>161</v>
+      <c r="B5" s="45" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -7299,10 +7421,10 @@
       <c r="Z9" s="3"/>
     </row>
     <row r="10" spans="1:26" ht="53.5" customHeight="1" x14ac:dyDescent="1.95">
-      <c r="A10" s="61" t="s">
+      <c r="A10" s="73" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="62"/>
+      <c r="B10" s="74"/>
       <c r="C10" s="14">
         <f>SUM(C2:C9)</f>
         <v>114</v>
@@ -35062,7 +35184,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView zoomScale="40" workbookViewId="0">
@@ -35130,7 +35252,7 @@
         <v>105</v>
       </c>
       <c r="D2" s="42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E2" s="4">
         <v>0</v>
@@ -35171,7 +35293,7 @@
         <v>104</v>
       </c>
       <c r="D3" s="42" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E3" s="4">
         <v>0</v>
@@ -35212,7 +35334,7 @@
         <v>106</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E4" s="4">
         <v>0</v>
@@ -35253,7 +35375,7 @@
         <v>71</v>
       </c>
       <c r="D5" s="42" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E5" s="4">
         <v>5</v>
@@ -35294,7 +35416,7 @@
         <v>74</v>
       </c>
       <c r="D6" s="42" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E6" s="4">
         <v>8</v>
@@ -35335,7 +35457,7 @@
         <v>77</v>
       </c>
       <c r="D7" s="43" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E7" s="4">
         <v>9</v>
@@ -35376,7 +35498,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="42" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E8" s="4">
         <v>9</v>
@@ -35417,7 +35539,7 @@
         <v>82</v>
       </c>
       <c r="D9" s="42" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E9" s="4">
         <v>6</v>
@@ -35458,7 +35580,7 @@
         <v>85</v>
       </c>
       <c r="D10" s="42" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E10" s="4">
         <v>6</v>
@@ -35499,7 +35621,7 @@
         <v>87</v>
       </c>
       <c r="D11" s="42" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E11" s="4">
         <v>6</v>
@@ -35540,7 +35662,7 @@
         <v>136</v>
       </c>
       <c r="D12" s="42" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E12" s="4">
         <v>6</v>
@@ -35581,7 +35703,7 @@
         <v>91</v>
       </c>
       <c r="D13" s="42" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E13" s="4">
         <v>2</v>
@@ -35622,7 +35744,7 @@
         <v>94</v>
       </c>
       <c r="D14" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E14" s="4">
         <v>2</v>
@@ -35663,7 +35785,7 @@
         <v>96</v>
       </c>
       <c r="D15" s="42" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E15" s="4">
         <v>3</v>
@@ -35704,7 +35826,7 @@
         <v>99</v>
       </c>
       <c r="D16" s="42" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E16" s="4">
         <v>8</v>
@@ -63300,6 +63422,5 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
   <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Merge pull request #50 from kku-computer-science/kunyakon_2622"
This reverts commit 21c6f5003505dd8e7b8a3792cf025382723b99a5, reversing
changes made to d5df41f694d413813ab53486ccb7562a5c48e2f7.
</commit_message>
<xml_diff>
--- a/docs/Excel_sprint1.xlsx
+++ b/docs/Excel_sprint1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sprint1\git-group-repository-group-3-sec-2-v-2\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D359F6D0-770A-4165-B7C8-DC963F9E5743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{592D4D6E-B802-42BD-849A-ADAB2E9CA726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -467,6 +467,9 @@
 https://sesec2group3.cpkkuhost.com</t>
   </si>
   <si>
+    <t>SESec2Group3</t>
+  </si>
+  <si>
     <t xml:space="preserve">DATE: </t>
   </si>
   <si>
@@ -552,9 +555,6 @@
   </si>
   <si>
     <t>เนื่องจากหน้าก่อนหน้าเทสไม่สำเร็จ จึงส่งผลต่อหน้านี้ด้วย</t>
-  </si>
-  <si>
-    <t>SESec2Group3_Sprint1</t>
   </si>
 </sst>
 </file>
@@ -977,42 +977,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1065,6 +1029,42 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2448,128 +2448,6 @@
     </xdr:pic>
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>6350</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>273050</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>635000</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="image4.jpg">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22504314-3D0D-C796-4F01-369E05A74BD8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="19634200" y="0"/>
-          <a:ext cx="3289300" cy="4876800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>6350</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>273050</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>635000</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F162D8E-9A64-E35F-5FA2-B4483096B987}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="19634200" y="0"/>
-          <a:ext cx="3289300" cy="4876800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2814,12 +2692,12 @@
         <v>5</v>
       </c>
       <c r="I3" s="23" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
-      <c r="J3" s="56" t="s">
+      <c r="J3" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="57"/>
+      <c r="K3" s="45"/>
     </row>
     <row r="4" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3818,7 +3696,7 @@
   <dimension ref="A1:I997"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="53" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C4"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.95"/>
@@ -3834,14 +3712,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="1.55">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="68"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="56"/>
       <c r="I1" s="20" t="s">
         <v>8</v>
       </c>
@@ -3861,54 +3739,54 @@
       <c r="A3" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="69" t="s">
-        <v>170</v>
+      <c r="B3" s="57" t="s">
+        <v>141</v>
       </c>
-      <c r="C3" s="65"/>
+      <c r="C3" s="53"/>
       <c r="D3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="64"/>
-      <c r="F3" s="57"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="45"/>
     </row>
     <row r="4" spans="1:9" ht="44.5" customHeight="1" x14ac:dyDescent="0.95">
       <c r="A4" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="70"/>
-      <c r="C4" s="65"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="53"/>
       <c r="D4" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="71">
+      <c r="E4" s="59">
         <f ca="1">TODAY()</f>
-        <v>45713</v>
+        <v>45700</v>
       </c>
-      <c r="F4" s="57"/>
+      <c r="F4" s="45"/>
     </row>
     <row r="5" spans="1:9" ht="36.5" customHeight="1" x14ac:dyDescent="0.95">
       <c r="A5" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="64"/>
-      <c r="C5" s="65"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="53"/>
       <c r="D5" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="72" t="s">
+      <c r="E5" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="57"/>
+      <c r="F5" s="45"/>
     </row>
     <row r="6" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="57"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="45"/>
     </row>
     <row r="7" spans="1:9" ht="32.5" customHeight="1" x14ac:dyDescent="0.95">
       <c r="A7" s="8"/>
@@ -3939,7 +3817,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="107" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A9" s="58" t="s">
+      <c r="A9" s="46" t="s">
         <v>124</v>
       </c>
       <c r="B9" s="25" t="s">
@@ -3952,14 +3830,14 @@
         <v>109</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="93.5" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A10" s="59"/>
+      <c r="A10" s="47"/>
       <c r="B10" s="27" t="s">
         <v>25</v>
       </c>
@@ -3973,11 +3851,11 @@
         <v>111</v>
       </c>
       <c r="F10" s="26" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="146" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A11" s="59"/>
+      <c r="A11" s="47"/>
       <c r="B11" s="25" t="s">
         <v>26</v>
       </c>
@@ -3991,11 +3869,11 @@
         <v>112</v>
       </c>
       <c r="F11" s="26" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="106.5" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A12" s="59"/>
+      <c r="A12" s="47"/>
       <c r="B12" s="25" t="s">
         <v>27</v>
       </c>
@@ -4014,7 +3892,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="125" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A13" s="59"/>
+      <c r="A13" s="47"/>
       <c r="B13" s="25" t="s">
         <v>28</v>
       </c>
@@ -4033,7 +3911,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="88" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A14" s="59"/>
+      <c r="A14" s="47"/>
       <c r="B14" s="25" t="s">
         <v>29</v>
       </c>
@@ -4044,7 +3922,7 @@
         <v>137</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F14" s="26" t="str">
         <f t="shared" si="0"/>
@@ -4052,7 +3930,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="156.5" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A15" s="59"/>
+      <c r="A15" s="47"/>
       <c r="B15" s="25" t="s">
         <v>30</v>
       </c>
@@ -4063,7 +3941,7 @@
         <v>119</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F15" s="26" t="str">
         <f t="shared" si="0"/>
@@ -4071,7 +3949,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="219.5" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A16" s="59"/>
+      <c r="A16" s="47"/>
       <c r="B16" s="25" t="s">
         <v>31</v>
       </c>
@@ -4082,7 +3960,7 @@
         <v>121</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F16" s="26" t="str">
         <f t="shared" si="0"/>
@@ -4090,7 +3968,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="105.5" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A17" s="59"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="25" t="s">
         <v>32</v>
       </c>
@@ -4101,7 +3979,7 @@
         <v>126</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F17" s="26" t="str">
         <f t="shared" si="0"/>
@@ -4109,18 +3987,18 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="104" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A18" s="59"/>
+      <c r="A18" s="47"/>
       <c r="B18" s="25" t="s">
         <v>33</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D18" s="35" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E18" s="35" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F18" s="26" t="str">
         <f t="shared" ref="F18" si="1">IF(E18="","",IF(D18=E18,"Pass","Fail"))</f>
@@ -4128,19 +4006,19 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="2.5" hidden="1" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A19" s="59"/>
+      <c r="A19" s="47"/>
     </row>
     <row r="20" spans="1:6" ht="32.5" hidden="1" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A20" s="59"/>
+      <c r="A20" s="47"/>
     </row>
     <row r="21" spans="1:6" ht="42" hidden="1" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A21" s="59"/>
+      <c r="A21" s="47"/>
     </row>
     <row r="22" spans="1:6" ht="1" hidden="1" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A22" s="59"/>
+      <c r="A22" s="47"/>
     </row>
     <row r="23" spans="1:6" ht="3" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A23" s="60"/>
+      <c r="A23" s="48"/>
     </row>
     <row r="24" spans="1:6" ht="21.5" customHeight="1" x14ac:dyDescent="0.95"/>
     <row r="25" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.95">
@@ -4151,7 +4029,7 @@
       <c r="F25" s="31"/>
     </row>
     <row r="26" spans="1:6" ht="89.5" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A26" s="61" t="s">
+      <c r="A26" s="49" t="s">
         <v>138</v>
       </c>
       <c r="B26" s="37" t="s">
@@ -4164,14 +4042,14 @@
         <v>109</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F26" s="26" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="213.5" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A27" s="62"/>
+      <c r="A27" s="50"/>
       <c r="B27" s="37" t="s">
         <v>35</v>
       </c>
@@ -4184,17 +4062,17 @@
       <c r="E27" s="39" t="s">
         <v>127</v>
       </c>
-      <c r="F27" s="49" t="str">
-        <f t="shared" ref="F27" si="2">IF(E27="","",IF(D27=E27,"Pass","Fail"))</f>
+      <c r="F27" s="68" t="str">
+        <f t="shared" ref="F27:F32" si="2">IF(E27="","",IF(D27=E27,"Pass","Fail"))</f>
         <v>Pass</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="95.5" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A28" s="62"/>
-      <c r="B28" s="47" t="s">
+      <c r="A28" s="50"/>
+      <c r="B28" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="48" t="s">
+      <c r="C28" s="67" t="s">
         <v>135</v>
       </c>
       <c r="D28" s="40" t="s">
@@ -4203,17 +4081,17 @@
       <c r="E28" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="F28" s="54" t="s">
-        <v>162</v>
+      <c r="F28" s="73" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="115.5" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A29" s="62"/>
-      <c r="B29" s="53" t="s">
+      <c r="A29" s="50"/>
+      <c r="B29" s="72" t="s">
         <v>37</v>
       </c>
       <c r="C29" s="41" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D29" s="40" t="s">
         <v>130</v>
@@ -4221,30 +4099,30 @@
       <c r="E29" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="F29" s="55" t="s">
-        <v>162</v>
+      <c r="F29" s="74" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="99" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A30" s="62"/>
-      <c r="B30" s="50" t="s">
+      <c r="A30" s="50"/>
+      <c r="B30" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="51" t="s">
+      <c r="C30" s="70" t="s">
         <v>129</v>
       </c>
-      <c r="D30" s="52" t="s">
+      <c r="D30" s="71" t="s">
         <v>128</v>
       </c>
-      <c r="E30" s="52" t="s">
+      <c r="E30" s="71" t="s">
         <v>128</v>
       </c>
       <c r="F30" s="30" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="129" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A31" s="62"/>
+      <c r="A31" s="50"/>
       <c r="B31" s="37" t="s">
         <v>39</v>
       </c>
@@ -4258,16 +4136,16 @@
         <v>132</v>
       </c>
       <c r="F31" s="26" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="161" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A32" s="62"/>
+      <c r="A32" s="50"/>
       <c r="B32" s="37" t="s">
         <v>40</v>
       </c>
       <c r="C32" s="30" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D32" s="34" t="s">
         <v>133</v>
@@ -4276,47 +4154,47 @@
         <v>133</v>
       </c>
       <c r="F32" s="26" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A33" s="62"/>
+      <c r="A33" s="50"/>
       <c r="B33" s="37" t="s">
         <v>123</v>
       </c>
       <c r="C33" s="30" t="s">
+        <v>164</v>
+      </c>
+      <c r="D33" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="E33" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="F33" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="D33" s="34" t="s">
-        <v>164</v>
-      </c>
-      <c r="E33" s="34" t="s">
-        <v>164</v>
-      </c>
-      <c r="F33" s="26" t="s">
-        <v>162</v>
-      </c>
     </row>
     <row r="34" spans="1:6" ht="76" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A34" s="62"/>
+      <c r="A34" s="50"/>
       <c r="B34" s="37" t="s">
         <v>134</v>
       </c>
       <c r="C34" s="30" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D34" s="34" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E34" s="26" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F34" s="26" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="92.5" hidden="1" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A35" s="62"/>
+      <c r="A35" s="50"/>
       <c r="B35" s="31"/>
       <c r="C35" s="31"/>
       <c r="D35" s="31"/>
@@ -4324,7 +4202,7 @@
       <c r="F35" s="31"/>
     </row>
     <row r="36" spans="1:6" ht="78" hidden="1" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A36" s="62"/>
+      <c r="A36" s="50"/>
       <c r="B36" s="31"/>
       <c r="C36" s="31"/>
       <c r="D36" s="31"/>
@@ -4332,7 +4210,7 @@
       <c r="F36" s="31"/>
     </row>
     <row r="37" spans="1:6" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A37" s="62"/>
+      <c r="A37" s="50"/>
       <c r="B37" s="31"/>
       <c r="C37" s="31"/>
       <c r="D37" s="31"/>
@@ -4340,7 +4218,7 @@
       <c r="F37" s="31"/>
     </row>
     <row r="38" spans="1:6" ht="82.5" hidden="1" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A38" s="62"/>
+      <c r="A38" s="50"/>
       <c r="B38" s="31"/>
       <c r="C38" s="31"/>
       <c r="D38" s="31"/>
@@ -4348,7 +4226,7 @@
       <c r="F38" s="31"/>
     </row>
     <row r="39" spans="1:6" ht="0.5" customHeight="1" x14ac:dyDescent="1.25">
-      <c r="A39" s="62"/>
+      <c r="A39" s="50"/>
       <c r="B39" s="32"/>
       <c r="C39" s="32"/>
       <c r="D39" s="32"/>
@@ -4356,7 +4234,7 @@
       <c r="F39" s="32"/>
     </row>
     <row r="40" spans="1:6" ht="1" customHeight="1" x14ac:dyDescent="1.25">
-      <c r="A40" s="62"/>
+      <c r="A40" s="50"/>
       <c r="B40" s="32"/>
       <c r="C40" s="32"/>
       <c r="D40" s="32"/>
@@ -4364,7 +4242,7 @@
       <c r="F40" s="32"/>
     </row>
     <row r="41" spans="1:6" ht="1.5" customHeight="1" x14ac:dyDescent="1.25">
-      <c r="A41" s="62"/>
+      <c r="A41" s="50"/>
       <c r="B41" s="32"/>
       <c r="C41" s="32"/>
       <c r="D41" s="32"/>
@@ -7052,43 +6930,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="44">
+      <c r="A1" s="63">
         <v>45693</v>
       </c>
-      <c r="B1" s="46" t="s">
-        <v>157</v>
+      <c r="B1" s="65" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="51.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="44">
+      <c r="A2" s="63">
         <v>45694</v>
       </c>
-      <c r="B2" s="46" t="s">
-        <v>158</v>
+      <c r="B2" s="65" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="44">
+      <c r="A3" s="63">
         <v>45695</v>
       </c>
-      <c r="B3" s="45" t="s">
-        <v>159</v>
+      <c r="B3" s="64" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="44">
+      <c r="A4" s="63">
         <v>45698</v>
       </c>
-      <c r="B4" s="45" t="s">
-        <v>159</v>
+      <c r="B4" s="64" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="44">
+      <c r="A5" s="63">
         <v>45699</v>
       </c>
-      <c r="B5" s="45" t="s">
-        <v>160</v>
+      <c r="B5" s="64" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -7421,10 +7299,10 @@
       <c r="Z9" s="3"/>
     </row>
     <row r="10" spans="1:26" ht="53.5" customHeight="1" x14ac:dyDescent="1.95">
-      <c r="A10" s="73" t="s">
+      <c r="A10" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="74"/>
+      <c r="B10" s="62"/>
       <c r="C10" s="14">
         <f>SUM(C2:C9)</f>
         <v>114</v>
@@ -35184,7 +35062,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView zoomScale="40" workbookViewId="0">
@@ -35252,7 +35130,7 @@
         <v>105</v>
       </c>
       <c r="D2" s="42" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E2" s="4">
         <v>0</v>
@@ -35293,7 +35171,7 @@
         <v>104</v>
       </c>
       <c r="D3" s="42" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E3" s="4">
         <v>0</v>
@@ -35334,7 +35212,7 @@
         <v>106</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E4" s="4">
         <v>0</v>
@@ -35375,7 +35253,7 @@
         <v>71</v>
       </c>
       <c r="D5" s="42" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E5" s="4">
         <v>5</v>
@@ -35416,7 +35294,7 @@
         <v>74</v>
       </c>
       <c r="D6" s="42" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E6" s="4">
         <v>8</v>
@@ -35457,7 +35335,7 @@
         <v>77</v>
       </c>
       <c r="D7" s="43" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E7" s="4">
         <v>9</v>
@@ -35498,7 +35376,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="42" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E8" s="4">
         <v>9</v>
@@ -35539,7 +35417,7 @@
         <v>82</v>
       </c>
       <c r="D9" s="42" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E9" s="4">
         <v>6</v>
@@ -35580,7 +35458,7 @@
         <v>85</v>
       </c>
       <c r="D10" s="42" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E10" s="4">
         <v>6</v>
@@ -35621,7 +35499,7 @@
         <v>87</v>
       </c>
       <c r="D11" s="42" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E11" s="4">
         <v>6</v>
@@ -35662,7 +35540,7 @@
         <v>136</v>
       </c>
       <c r="D12" s="42" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E12" s="4">
         <v>6</v>
@@ -35703,7 +35581,7 @@
         <v>91</v>
       </c>
       <c r="D13" s="42" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E13" s="4">
         <v>2</v>
@@ -35744,7 +35622,7 @@
         <v>94</v>
       </c>
       <c r="D14" s="42" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E14" s="4">
         <v>2</v>
@@ -35785,7 +35663,7 @@
         <v>96</v>
       </c>
       <c r="D15" s="42" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E15" s="4">
         <v>3</v>
@@ -35826,7 +35704,7 @@
         <v>99</v>
       </c>
       <c r="D16" s="42" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E16" s="4">
         <v>8</v>
@@ -63422,5 +63300,6 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>